<commit_message>
File path Changes.. and some minore changes also
</commit_message>
<xml_diff>
--- a/media/BAJAJ-PL/MIS/BAJAJ-PL MIS.xlsx
+++ b/media/BAJAJ-PL/MIS/BAJAJ-PL MIS.xlsx
@@ -466,7 +466,7 @@
         <v>694841</v>
       </c>
       <c r="D2" t="n">
-        <v>3.498821906203006</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>37918778.37000001</v>
+        <v>37918778.37</v>
       </c>
       <c r="C3" t="n">
         <v>547840</v>
       </c>
       <c r="D3" t="n">
-        <v>1.444772283153066</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>33571278.87999998</v>
+        <v>33571278.88</v>
       </c>
       <c r="C4" t="n">
         <v>196362</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5849106931609396</v>
+        <v>0.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>